<commit_message>
revisione coibentazione delle tubazioni
</commit_message>
<xml_diff>
--- a/FogliCalcolo/Piping/Coibentazione delle tubazioni.xlsx
+++ b/FogliCalcolo/Piping/Coibentazione delle tubazioni.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Uni\Impianti meccanici\MaterialeEsame\FogliCalcolo\Piping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giona\Desktop\git\ImpiantiMeccanici\FogliCalcolo\Piping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A75C09C-2E78-4DF3-9A30-8C75571A1E4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69B0275-DCD4-4E6E-8008-544AF63EEDA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antistillicidio" sheetId="1" r:id="rId1"/>
-    <sheet name="coibente" sheetId="6" r:id="rId2"/>
+    <sheet name="Coibente" sheetId="6" r:id="rId2"/>
     <sheet name="Antigelo" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="84">
   <si>
     <t>Fluido</t>
   </si>
@@ -163,9 +163,6 @@
     <t xml:space="preserve">Potenza dispersa </t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>re</t>
   </si>
   <si>
@@ -217,15 +214,9 @@
     <t>Temperatura mantello in funzione della lunghezza</t>
   </si>
   <si>
-    <t>G</t>
-  </si>
-  <si>
     <t>ri</t>
   </si>
   <si>
-    <t>v</t>
-  </si>
-  <si>
     <t>tin</t>
   </si>
   <si>
@@ -238,15 +229,6 @@
     <t>s [m]</t>
   </si>
   <si>
-    <t>s               [m]</t>
-  </si>
-  <si>
-    <t>R               [m °C/W]</t>
-  </si>
-  <si>
-    <t>tout           [°C]</t>
-  </si>
-  <si>
     <t>he</t>
   </si>
   <si>
@@ -263,9 +245,6 @@
   </si>
   <si>
     <t xml:space="preserve">v </t>
-  </si>
-  <si>
-    <t>st</t>
   </si>
   <si>
     <t>λis</t>
@@ -317,16 +296,70 @@
   <si>
     <t>Te [°C]</t>
   </si>
+  <si>
+    <t>Spessore tubo</t>
+  </si>
+  <si>
+    <t>spessore tubo</t>
+  </si>
+  <si>
+    <t>raggio esterno</t>
+  </si>
+  <si>
+    <t>lunghezza tubo</t>
+  </si>
+  <si>
+    <t>raggio interno</t>
+  </si>
+  <si>
+    <t>velocità</t>
+  </si>
+  <si>
+    <t>portata massica</t>
+  </si>
+  <si>
+    <t>temperatura uscita fluido</t>
+  </si>
+  <si>
+    <t>temperatura ingresso fluido</t>
+  </si>
+  <si>
+    <t>temperatura ambiente</t>
+  </si>
+  <si>
+    <t>λisolante</t>
+  </si>
+  <si>
+    <t>coefficiente di adduzione he</t>
+  </si>
+  <si>
+    <t>[m]</t>
+  </si>
+  <si>
+    <t>[m °C/W]</t>
+  </si>
+  <si>
+    <t>[°C]</t>
+  </si>
+  <si>
+    <t>spessore isolante</t>
+  </si>
+  <si>
+    <t>spessore</t>
+  </si>
+  <si>
+    <t>portata</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -522,10 +555,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -535,9 +568,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -578,26 +608,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -605,40 +620,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -651,7 +645,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -659,16 +653,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -686,10 +680,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
@@ -776,7 +852,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>coibente!$B$35:$B$65</c:f>
+              <c:f>Coibente!$B$36:$B$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -878,7 +954,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>coibente!$C$35:$C$65</c:f>
+              <c:f>Coibente!$C$36:$C$66</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
@@ -1068,7 +1144,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="it-IT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1106,7 +1182,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="287040415"/>
@@ -1186,7 +1262,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="it-IT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1224,7 +1300,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="287039999"/>
@@ -1265,7 +1341,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1840,14 +1916,14 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>314325</xdr:colOff>
-          <xdr:row>10</xdr:row>
+          <xdr:row>11</xdr:row>
           <xdr:rowOff>85725</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>2932</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>371475</xdr:rowOff>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1857,7 +1933,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDD5CEFD-163A-481A-A510-280C0C615F75}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1895,13 +1971,13 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>13</xdr:row>
+          <xdr:row>14</xdr:row>
           <xdr:rowOff>95250</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>2819400</xdr:colOff>
-          <xdr:row>13</xdr:row>
+          <xdr:row>14</xdr:row>
           <xdr:rowOff>819150</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1912,7 +1988,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71E0A3A7-E24C-48EE-A8F4-50AC6A39EBDC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1953,15 +2029,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>488260</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>13252</xdr:rowOff>
+          <xdr:colOff>485775</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1964635</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>299002</xdr:rowOff>
+          <xdr:colOff>1962150</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1971,7 +2047,7 @@
                   <a14:compatExt spid="_x0000_s6145"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5DE3B9F-2BE6-4BE8-B343-2C01A87FBDA2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2009,13 +2085,13 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>15</xdr:row>
+          <xdr:row>16</xdr:row>
           <xdr:rowOff>95250</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>2819400</xdr:colOff>
-          <xdr:row>15</xdr:row>
+          <xdr:row>16</xdr:row>
           <xdr:rowOff>819150</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2026,7 +2102,7 @@
                   <a14:compatExt spid="_x0000_s6146"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E37C34C-E4F2-4680-9394-D31BA442CDD8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2063,13 +2139,13 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>18</xdr:row>
+          <xdr:row>19</xdr:row>
           <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>2809875</xdr:colOff>
-          <xdr:row>18</xdr:row>
+          <xdr:row>19</xdr:row>
           <xdr:rowOff>819150</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2080,7 +2156,7 @@
                   <a14:compatExt spid="_x0000_s6147"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65033A4B-2C20-4EC7-9189-868F2DD06955}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2117,13 +2193,13 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>18</xdr:row>
           <xdr:rowOff>57150</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>2695575</xdr:colOff>
-          <xdr:row>18</xdr:row>
+          <xdr:row>19</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2134,7 +2210,7 @@
                   <a14:compatExt spid="_x0000_s6148"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1D89B3C-EA59-4D15-B337-0F33A45D786E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2171,13 +2247,13 @@
         <xdr:from>
           <xdr:col>2</xdr:col>
           <xdr:colOff>361950</xdr:colOff>
-          <xdr:row>21</xdr:row>
+          <xdr:row>22</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>2657475</xdr:colOff>
-          <xdr:row>22</xdr:row>
+          <xdr:row>23</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2188,7 +2264,7 @@
                   <a14:compatExt spid="_x0000_s6149"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97EE736B-BF78-47E0-B6B1-C0D96E257A82}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2223,23 +2299,23 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1524785</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>154179</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="Object 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA511243-7B1B-4C39-97F5-6BE5FF3BAE78}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2271,7 +2347,7 @@
                       <m:accPr>
                         <m:chr m:val="̇"/>
                         <m:ctrlPr>
-                          <a:rPr lang="en-US">
+                          <a:rPr lang="en-US" i="1">
                             <a:solidFill>
                               <a:srgbClr val="000000"/>
                             </a:solidFill>
@@ -2401,13 +2477,12 @@
               </a:endParaRPr>
             </a:p>
             <a:p>
-              <a:pPr/>
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="Object 6">
@@ -2473,13 +2548,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2487,7 +2562,7 @@
         <xdr:cNvPr id="3" name="Grafico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC199133-6025-44A4-AEF7-8FD607A46F44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2829,10 +2904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H39"/>
+  <dimension ref="B1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2848,536 +2923,550 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="77" t="s">
         <v>1</v>
       </c>
+      <c r="E2" s="76"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16" t="s">
+      <c r="C3" s="14"/>
+      <c r="D3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="45">
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="16">
+        <v>3.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="58">
-        <f>+E5-0.0036</f>
+      <c r="E6" s="45">
+        <f>+E4-E5</f>
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="16">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="16">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="46">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="48"/>
+      <c r="D12" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="50">
+        <f>9.5+0.0085*E9^(4/3)</f>
+        <v>10.473142227281105</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="58">
-        <f>0.108/2</f>
-        <v>5.3999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="17">
+      <c r="E13" s="45">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="45">
+        <f>+E4+E13</f>
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="H14" s="65"/>
+    </row>
+    <row r="15" spans="2:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="63"/>
+      <c r="D15" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="90">
+        <f>+E9-(E9-E3)/(E12*E14/E8*LN(E14/E4)+1)</f>
+        <v>31.145496892137551</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="C19" s="58">
+        <f>+$E$4+B19</f>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="D19" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C19/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>30.630941967802464</v>
+      </c>
+      <c r="E19" s="16" t="str">
+        <f>IF(D19&gt;$E$11,"OK","NO")</f>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="33">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C20" s="58">
+        <f t="shared" ref="C20:C39" si="0">+$E$4+B20</f>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="D20" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C20/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>30.744557590150563</v>
+      </c>
+      <c r="E20" s="16" t="str">
+        <f t="shared" ref="E20:E39" si="1">IF(D20&gt;$E$11,"OK","NO")</f>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="33">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C21" s="58">
+        <f t="shared" si="0"/>
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="D21" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C21/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>30.852413922112468</v>
+      </c>
+      <c r="E21" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="33">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C22" s="58">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D22" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C22/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>30.954938055188784</v>
+      </c>
+      <c r="E22" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="33">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="C23" s="58">
+        <f t="shared" si="0"/>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="D23" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C23/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>31.052515870479773</v>
+      </c>
+      <c r="E23" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="C24" s="58">
+        <f t="shared" si="0"/>
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="D24" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C24/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>31.145496892137551</v>
+      </c>
+      <c r="E24" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="33">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C25" s="58">
+        <f t="shared" si="0"/>
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="D25" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C25/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>31.234198470679228</v>
+      </c>
+      <c r="E25" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="33">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C26" s="58">
+        <f t="shared" si="0"/>
+        <v>7.8E-2</v>
+      </c>
+      <c r="D26" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C26/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>31.318909401683428</v>
+      </c>
+      <c r="E26" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="33">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="C27" s="58">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+      <c r="D27" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C27/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>31.399893066820795</v>
+      </c>
+      <c r="E27" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="33">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="C28" s="58">
+        <f t="shared" si="0"/>
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D28" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C28/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>31.477390169195274</v>
+      </c>
+      <c r="E28" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="33">
+        <v>0.03</v>
+      </c>
+      <c r="C29" s="58">
+        <f t="shared" si="0"/>
+        <v>8.3999999999999991E-2</v>
+      </c>
+      <c r="D29" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C29/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>31.551621122839016</v>
+      </c>
+      <c r="E29" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="33">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C30" s="58">
+        <f t="shared" si="0"/>
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="D30" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C30/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>31.622788146323444</v>
+      </c>
+      <c r="E30" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="33">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="C31" s="58">
+        <f t="shared" si="0"/>
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="D31" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C31/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>31.691077102367011</v>
+      </c>
+      <c r="E31" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="33">
         <v>3.5999999999999997E-2</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="17">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="59">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="63">
-        <f>9.5+0.0085*E8^(4/3)</f>
-        <v>10.473142227281105</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="58">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="58">
-        <f>+E5+E12</f>
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="H13" s="79"/>
-    </row>
-    <row r="14" spans="2:8" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="75" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="76"/>
-      <c r="D14" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="78">
-        <f>+E8+-(E8-E3)/(E11*E13/E7*LN(E13/E5)+1)</f>
-        <v>31.145496892137551</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="39">
-        <v>0.01</v>
-      </c>
-      <c r="C18" s="71">
-        <f>+$E$5+B18</f>
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="D18" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C18/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>30.630941967802464</v>
-      </c>
-      <c r="E18" s="17" t="str">
-        <f>IF(D18&gt;$E$10,"OK","NO")</f>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="39">
-        <v>1.2E-2</v>
-      </c>
-      <c r="C19" s="71">
-        <f>+$E$5+B19</f>
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="D19" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C19/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>30.744557590150563</v>
-      </c>
-      <c r="E19" s="17" t="str">
-        <f t="shared" ref="E19:E38" si="0">IF(D19&gt;$E$10,"OK","NO")</f>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="39">
-        <v>1.4E-2</v>
-      </c>
-      <c r="C20" s="71">
-        <f>+$E$5+B20</f>
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="D20" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C20/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>30.852413922112468</v>
-      </c>
-      <c r="E20" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="39">
-        <v>1.6E-2</v>
-      </c>
-      <c r="C21" s="71">
-        <f>+$E$5+B21</f>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D21" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C21/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>30.954938055188784</v>
-      </c>
-      <c r="E21" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="39">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="C22" s="71">
-        <f>+$E$5+B22</f>
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="D22" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C22/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>31.052515870479773</v>
-      </c>
-      <c r="E22" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="C32" s="58">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="D32" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C32/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>31.756659118679575</v>
+      </c>
+      <c r="E32" s="16" t="str">
+        <f t="shared" si="1"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="39">
-        <v>0.02</v>
-      </c>
-      <c r="C23" s="71">
-        <f>+$E$5+B23</f>
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="D23" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C23/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>31.145496892137551</v>
-      </c>
-      <c r="E23" s="17" t="str">
-        <f t="shared" si="0"/>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="33">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C33" s="58">
+        <f t="shared" si="0"/>
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="D33" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C33/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>31.819692019804396</v>
+      </c>
+      <c r="E33" s="16" t="str">
+        <f t="shared" si="1"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="39">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="C24" s="71">
-        <f>+$E$5+B24</f>
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="D24" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C24/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>31.234198470679228</v>
-      </c>
-      <c r="E24" s="17" t="str">
-        <f t="shared" si="0"/>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="33">
+        <v>0.04</v>
+      </c>
+      <c r="C34" s="58">
+        <f t="shared" si="0"/>
+        <v>9.4E-2</v>
+      </c>
+      <c r="D34" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C34/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>31.88032159517984</v>
+      </c>
+      <c r="E34" s="16" t="str">
+        <f t="shared" si="1"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="39">
-        <v>2.4E-2</v>
-      </c>
-      <c r="C25" s="71">
-        <f>+$E$5+B25</f>
-        <v>7.8E-2</v>
-      </c>
-      <c r="D25" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C25/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>31.318909401683428</v>
-      </c>
-      <c r="E25" s="17" t="str">
-        <f t="shared" si="0"/>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="33">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C35" s="58">
+        <f t="shared" si="0"/>
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="D35" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C35/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>31.938682724868087</v>
+      </c>
+      <c r="E35" s="16" t="str">
+        <f t="shared" si="1"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="39">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="C26" s="71">
-        <f>+$E$5+B26</f>
-        <v>0.08</v>
-      </c>
-      <c r="D26" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C26/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>31.399893066820795</v>
-      </c>
-      <c r="E26" s="17" t="str">
-        <f t="shared" si="0"/>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="33">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="C36" s="58">
+        <f t="shared" si="0"/>
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="D36" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C36/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>31.99490038124739</v>
+      </c>
+      <c r="E36" s="16" t="str">
+        <f t="shared" si="1"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="39">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="C27" s="71">
-        <f>+$E$5+B27</f>
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="D27" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C27/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>31.477390169195274</v>
-      </c>
-      <c r="E27" s="17" t="str">
-        <f t="shared" si="0"/>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="33">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="C37" s="58">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="D37" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C37/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>32.049090522324889</v>
+      </c>
+      <c r="E37" s="16" t="str">
+        <f t="shared" si="1"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="39">
-        <v>0.03</v>
-      </c>
-      <c r="C28" s="71">
-        <f>+$E$5+B28</f>
-        <v>8.3999999999999991E-2</v>
-      </c>
-      <c r="D28" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C28/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>31.551621122839016</v>
-      </c>
-      <c r="E28" s="17" t="str">
-        <f t="shared" si="0"/>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="33">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="C38" s="58">
+        <f t="shared" si="0"/>
+        <v>0.10200000000000001</v>
+      </c>
+      <c r="D38" s="60">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C38/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>32.101360890108225</v>
+      </c>
+      <c r="E38" s="16" t="str">
+        <f t="shared" si="1"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="39">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="C29" s="71">
-        <f>+$E$5+B29</f>
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="D29" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C29/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>31.622788146323444</v>
-      </c>
-      <c r="E29" s="17" t="str">
-        <f t="shared" si="0"/>
+    <row r="39" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="C39" s="59">
+        <f t="shared" si="0"/>
+        <v>0.10400000000000001</v>
+      </c>
+      <c r="D39" s="61">
+        <f>+$E$9+-+($E$9-$E$3)/($E$12*C39/$E$8*LN($E$14/$E$4)+1)</f>
+        <v>32.15181172560326</v>
+      </c>
+      <c r="E39" s="29" t="str">
+        <f t="shared" si="1"/>
         <v>OK</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="39">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="C30" s="71">
-        <f>+$E$5+B30</f>
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="D30" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C30/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>31.691077102367011</v>
-      </c>
-      <c r="E30" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="39">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="C31" s="71">
-        <f>+$E$5+B31</f>
-        <v>0.09</v>
-      </c>
-      <c r="D31" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C31/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>31.756659118679575</v>
-      </c>
-      <c r="E31" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="39">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="C32" s="71">
-        <f>+$E$5+B32</f>
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="D32" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C32/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>31.819692019804396</v>
-      </c>
-      <c r="E32" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="39">
-        <v>0.04</v>
-      </c>
-      <c r="C33" s="71">
-        <f>+$E$5+B33</f>
-        <v>9.4E-2</v>
-      </c>
-      <c r="D33" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C33/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>31.88032159517984</v>
-      </c>
-      <c r="E33" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="39">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="C34" s="71">
-        <f>+$E$5+B34</f>
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="D34" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C34/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>31.938682724868087</v>
-      </c>
-      <c r="E34" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="39">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="C35" s="71">
-        <f>+$E$5+B35</f>
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="D35" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C35/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>31.99490038124739</v>
-      </c>
-      <c r="E35" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="39">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="C36" s="71">
-        <f>+$E$5+B36</f>
-        <v>0.1</v>
-      </c>
-      <c r="D36" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C36/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>32.049090522324889</v>
-      </c>
-      <c r="E36" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="39">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="C37" s="71">
-        <f>+$E$5+B37</f>
-        <v>0.10200000000000001</v>
-      </c>
-      <c r="D37" s="73">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C37/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>32.101360890108225</v>
-      </c>
-      <c r="E37" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="44">
-        <v>0.05</v>
-      </c>
-      <c r="C38" s="72">
-        <f>+$E$5+B38</f>
-        <v>0.10400000000000001</v>
-      </c>
-      <c r="D38" s="74">
-        <f>+$E$8+-+($E$8-$E$3)/($E$11*C38/$E$7*LN($E$13/$E$5)+1)</f>
-        <v>32.15181172560326</v>
-      </c>
-      <c r="E38" s="35" t="str">
-        <f t="shared" si="0"/>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="15"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="14"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D18:D38">
+  <mergeCells count="1">
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D19:D39">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
-      <formula>$E$10</formula>
+      <formula>$E$11</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3393,13 +3482,13 @@
               <from>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>314325</xdr:colOff>
-                <xdr:row>10</xdr:row>
+                <xdr:row>11</xdr:row>
                 <xdr:rowOff>85725</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>11</xdr:row>
+                <xdr:row>12</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
@@ -3418,13 +3507,13 @@
               <from>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>13</xdr:row>
+                <xdr:row>14</xdr:row>
                 <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>2819400</xdr:colOff>
-                <xdr:row>13</xdr:row>
+                <xdr:row>14</xdr:row>
                 <xdr:rowOff>819150</xdr:rowOff>
               </to>
             </anchor>
@@ -3441,10 +3530,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B05ACF0-4054-40A1-8772-F30D66E85C7E}">
-  <dimension ref="B1:H65"/>
+  <dimension ref="B1:H66"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3452,789 +3541,802 @@
     <col min="1" max="1" width="3.42578125" customWidth="1"/>
     <col min="2" max="2" width="33.28515625" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="56"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="68"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17" t="s">
+      <c r="C3" s="14"/>
+      <c r="D3" s="89" t="s">
         <v>19</v>
       </c>
+      <c r="E3" s="88"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="57">
+      <c r="E4" s="44">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16" t="s">
+      <c r="C5" s="14"/>
+      <c r="D5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="57">
+      <c r="E5" s="44">
         <v>80</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="45">
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="45">
+        <v>3.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="58">
-        <f>+E7-0.0036</f>
+      <c r="E8" s="45">
+        <f>E6-E7</f>
         <v>5.04E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="89" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="88"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="16">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="44">
         <v>18</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16" t="s">
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="46">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" s="2" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="48"/>
+      <c r="D14" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="50">
+        <f>9.5+0.0085*E11^(4/3)</f>
+        <v>9.9009734333139612</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="52"/>
+      <c r="D15" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="58">
-        <f>0.108/2</f>
-        <v>5.3999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="17">
-        <v>4.3999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
+      <c r="E15" s="54">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="45">
+        <f>+E6+E15</f>
+        <v>0.11399999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="57">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="59">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="E17" s="50">
+        <f>+E11-(E11-E4)/(E14*E16/E10*LN(E16/E6)+1)</f>
+        <v>21.570023593713483</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="16">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="50">
+        <f>1/2/PI()*(1/E10*LN(E16/E6)+1/E14/E16)</f>
+        <v>2.8437983325582827</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="50">
+        <f>(E4-E11)*E18/E19</f>
+        <v>7595.4753024166193</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="55">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" s="2" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="48"/>
+      <c r="D22" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="56">
+        <f>+PI()*E8^2*E21*1000</f>
+        <v>11.970221992413974</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="48"/>
+      <c r="D23" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="50">
+        <f>+E22*4180*(E4-E5)</f>
+        <v>500355.27928290411</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="57">
+        <f>E20/E23</f>
+        <v>1.518016420912407E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="13"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="16">
+        <v>4186</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="17">
+        <f>E11+(E4-E11)/EXP(E18/(E27*E22*E19))</f>
+        <v>89.848575398302629</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="17">
+        <f>E4-E28</f>
+        <v>0.15142460169737149</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="17">
+        <f>E27*E29*E22</f>
+        <v>7587.4854038436652</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="20">
+        <f>ABS(E30-E20)/E30</f>
+        <v>1.0530364340347422E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="70"/>
+      <c r="D34" s="71"/>
+      <c r="F34" s="79" t="s">
+        <v>52</v>
+      </c>
+      <c r="G34" s="80"/>
+      <c r="H34" s="81"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="82"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="84"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="6">
+        <v>0</v>
+      </c>
+      <c r="C36" s="21">
+        <f>$E$11+($E$4-$E$11)/EXP(B36/($E$27*$E$22*$E$19))</f>
+        <v>90</v>
+      </c>
+      <c r="D36" s="28">
+        <f>+$E$11-($E$11-C36)/($E$14*$E$16/$E$10*LN($E$16/$E$6)+1)</f>
+        <v>21.570023593713483</v>
+      </c>
+      <c r="F36" s="82"/>
+      <c r="G36" s="83"/>
+      <c r="H36" s="84"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="6">
         <v>10</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" s="2" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="63">
-        <f>9.5+0.0085*E10^(4/3)</f>
-        <v>9.9009734333139612</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="64" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="65"/>
-      <c r="D14" s="66" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="67">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="58">
-        <f>+E7+E14</f>
-        <v>0.11399999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="61"/>
-      <c r="D16" s="62" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="63">
-        <f>+E10-(E10-E4)/(E13*E15/E9*LN(E15/E7)+1)</f>
-        <v>21.570023593713483</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="17">
+      <c r="C37" s="21">
+        <f t="shared" ref="C37:C66" si="0">$E$11+($E$4-$E$11)/EXP(B37/($E$27*$E$22*$E$19))</f>
+        <v>89.994947375382452</v>
+      </c>
+      <c r="D37" s="28">
+        <f t="shared" ref="D37:D66" si="1">+$E$11-($E$11-C37)/($E$14*$E$16/$E$10*LN($E$16/$E$6)+1)</f>
+        <v>21.569773066087166</v>
+      </c>
+      <c r="F37" s="82"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="84"/>
+    </row>
+    <row r="38" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="6">
+        <v>20</v>
+      </c>
+      <c r="C38" s="21">
+        <f t="shared" si="0"/>
+        <v>89.989895105334568</v>
+      </c>
+      <c r="D38" s="28">
+        <f t="shared" si="1"/>
+        <v>21.569522556041711</v>
+      </c>
+      <c r="F38" s="85"/>
+      <c r="G38" s="86"/>
+      <c r="H38" s="87"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="6">
+        <v>30</v>
+      </c>
+      <c r="C39" s="21">
+        <f t="shared" si="0"/>
+        <v>89.98484318983148</v>
+      </c>
+      <c r="D39" s="28">
+        <f t="shared" si="1"/>
+        <v>21.569272063575884</v>
+      </c>
+      <c r="F39" s="78"/>
+      <c r="G39" s="78"/>
+      <c r="H39" s="78"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="6">
+        <v>40</v>
+      </c>
+      <c r="C40" s="21">
+        <f t="shared" si="0"/>
+        <v>89.979791628848275</v>
+      </c>
+      <c r="D40" s="28">
+        <f t="shared" si="1"/>
+        <v>21.56902158868845</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="6">
+        <v>50</v>
+      </c>
+      <c r="C41" s="21">
+        <f t="shared" si="0"/>
+        <v>89.974740422360085</v>
+      </c>
+      <c r="D41" s="28">
+        <f t="shared" si="1"/>
+        <v>21.568771131378181</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="6">
+        <v>60</v>
+      </c>
+      <c r="C42" s="21">
+        <f t="shared" si="0"/>
+        <v>89.969689570342041</v>
+      </c>
+      <c r="D42" s="28">
+        <f t="shared" si="1"/>
+        <v>21.568520691643837</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="6">
+        <v>70</v>
+      </c>
+      <c r="C43" s="21">
+        <f t="shared" si="0"/>
+        <v>89.964639072769259</v>
+      </c>
+      <c r="D43" s="28">
+        <f t="shared" si="1"/>
+        <v>21.568270269484184</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="6">
+        <v>80</v>
+      </c>
+      <c r="C44" s="21">
+        <f t="shared" si="0"/>
+        <v>89.959588929616871</v>
+      </c>
+      <c r="D44" s="28">
+        <f t="shared" si="1"/>
+        <v>21.568019864897995</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="6">
+        <v>90</v>
+      </c>
+      <c r="C45" s="21">
+        <f t="shared" si="0"/>
+        <v>89.954539140860021</v>
+      </c>
+      <c r="D45" s="28">
+        <f t="shared" si="1"/>
+        <v>21.567769477884035</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="6">
+        <v>100</v>
+      </c>
+      <c r="C46" s="21">
+        <f t="shared" si="0"/>
+        <v>89.949489706473813</v>
+      </c>
+      <c r="D46" s="28">
+        <f t="shared" si="1"/>
+        <v>21.567519108441068</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="6">
+        <v>110</v>
+      </c>
+      <c r="C47" s="21">
+        <f t="shared" si="0"/>
+        <v>89.944440626433391</v>
+      </c>
+      <c r="D47" s="28">
+        <f t="shared" si="1"/>
+        <v>21.567268756567859</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="6">
+        <v>120</v>
+      </c>
+      <c r="C48" s="21">
+        <f t="shared" si="0"/>
+        <v>89.939391900713886</v>
+      </c>
+      <c r="D48" s="28">
+        <f t="shared" si="1"/>
+        <v>21.567018422263182</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="6">
+        <v>130</v>
+      </c>
+      <c r="C49" s="21">
+        <f t="shared" si="0"/>
+        <v>89.93434352929043</v>
+      </c>
+      <c r="D49" s="28">
+        <f t="shared" si="1"/>
+        <v>21.566768105525799</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="6">
+        <v>140</v>
+      </c>
+      <c r="C50" s="21">
+        <f t="shared" si="0"/>
+        <v>89.929295512138168</v>
+      </c>
+      <c r="D50" s="28">
+        <f t="shared" si="1"/>
+        <v>21.566517806354479</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="6">
+        <v>150</v>
+      </c>
+      <c r="C51" s="21">
+        <f t="shared" si="0"/>
+        <v>89.924247849232245</v>
+      </c>
+      <c r="D51" s="28">
+        <f t="shared" si="1"/>
+        <v>21.566267524747989</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="6">
+        <v>160</v>
+      </c>
+      <c r="C52" s="21">
+        <f t="shared" si="0"/>
+        <v>89.919200540547791</v>
+      </c>
+      <c r="D52" s="28">
+        <f t="shared" si="1"/>
+        <v>21.566017260705099</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="6">
+        <v>170</v>
+      </c>
+      <c r="C53" s="21">
+        <f t="shared" si="0"/>
+        <v>89.914153586059939</v>
+      </c>
+      <c r="D53" s="28">
+        <f t="shared" si="1"/>
+        <v>21.565767014224569</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="6">
+        <v>180</v>
+      </c>
+      <c r="C54" s="21">
+        <f t="shared" si="0"/>
+        <v>89.909106985743847</v>
+      </c>
+      <c r="D54" s="28">
+        <f t="shared" si="1"/>
+        <v>21.565516785305174</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="6">
+        <v>190</v>
+      </c>
+      <c r="C55" s="21">
+        <f t="shared" si="0"/>
+        <v>89.90406073957466</v>
+      </c>
+      <c r="D55" s="28">
+        <f t="shared" si="1"/>
+        <v>21.565266573945678</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="6">
+        <v>200</v>
+      </c>
+      <c r="C56" s="21">
+        <f t="shared" si="0"/>
+        <v>89.899014847527511</v>
+      </c>
+      <c r="D56" s="28">
+        <f t="shared" si="1"/>
+        <v>21.565016380144851</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="6">
+        <v>210</v>
+      </c>
+      <c r="C57" s="21">
+        <f t="shared" si="0"/>
+        <v>89.893969309577585</v>
+      </c>
+      <c r="D57" s="28">
+        <f t="shared" si="1"/>
+        <v>21.564766203901456</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="6">
+        <v>220</v>
+      </c>
+      <c r="C58" s="21">
+        <f t="shared" si="0"/>
+        <v>89.888924125700001</v>
+      </c>
+      <c r="D58" s="28">
+        <f t="shared" si="1"/>
+        <v>21.564516045214269</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="6">
+        <v>230</v>
+      </c>
+      <c r="C59" s="21">
+        <f t="shared" si="0"/>
+        <v>89.883879295869917</v>
+      </c>
+      <c r="D59" s="28">
+        <f t="shared" si="1"/>
+        <v>21.564265904082053</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="6">
+        <v>240</v>
+      </c>
+      <c r="C60" s="21">
+        <f t="shared" si="0"/>
+        <v>89.878834820062494</v>
+      </c>
+      <c r="D60" s="28">
+        <f t="shared" si="1"/>
+        <v>21.564015780503574</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="6">
+        <v>250</v>
+      </c>
+      <c r="C61" s="21">
+        <f t="shared" si="0"/>
+        <v>89.873790698252861</v>
+      </c>
+      <c r="D61" s="28">
+        <f t="shared" si="1"/>
+        <v>21.563765674477601</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="6">
+        <v>260</v>
+      </c>
+      <c r="C62" s="21">
+        <f t="shared" si="0"/>
+        <v>89.868746930416222</v>
+      </c>
+      <c r="D62" s="28">
+        <f t="shared" si="1"/>
+        <v>21.563515586002907</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="6">
+        <v>270</v>
+      </c>
+      <c r="C63" s="21">
+        <f t="shared" si="0"/>
+        <v>89.863703516527721</v>
+      </c>
+      <c r="D63" s="28">
+        <f t="shared" si="1"/>
+        <v>21.563265515078257</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="6">
+        <v>280</v>
+      </c>
+      <c r="C64" s="21">
+        <f t="shared" si="0"/>
+        <v>89.858660456562518</v>
+      </c>
+      <c r="D64" s="28">
+        <f t="shared" si="1"/>
+        <v>21.56301546170242</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="6">
+        <v>290</v>
+      </c>
+      <c r="C65" s="21">
+        <f t="shared" si="0"/>
+        <v>89.853617750495758</v>
+      </c>
+      <c r="D65" s="28">
+        <f t="shared" si="1"/>
+        <v>21.562765425874161</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="7">
         <v>300</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="60" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="63">
-        <f>1/2/PI()*(1/E9*LN(E15/E7)+1/E13/E15)</f>
-        <v>2.8437983325582827</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="60" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="61"/>
-      <c r="D19" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="63">
-        <f>(E4-E10)*E17/E18</f>
-        <v>7595.4753024166193</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="68">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" s="2" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="62" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="69">
-        <f>+PI()*E6^2*E20*1000</f>
-        <v>11.970221992413974</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="63">
-        <f>+E21*4180*(E4-E5)</f>
-        <v>500355.27928290411</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="70">
-        <f>E19/E22</f>
-        <v>1.518016420912407E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="14"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="17">
-        <v>4186</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="18">
-        <f>E10+(E4-E10)/EXP(E17/(E26*E21*E18))</f>
+      <c r="C66" s="22">
+        <f t="shared" si="0"/>
         <v>89.848575398302629</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28" s="18">
-        <f>E4-E27</f>
-        <v>0.15142460169737149</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="18">
-        <f>E26*E28*E21</f>
-        <v>7587.4854038436652</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21">
-        <f>ABS(E29-E19)/E29</f>
-        <v>1.0530364340347422E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
-      <c r="F33" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="7">
-        <v>0</v>
-      </c>
-      <c r="C35" s="22">
-        <f>$E$10+($E$4-$E$10)/EXP(B35/($E$26*$E$21*$E$18))</f>
-        <v>90</v>
-      </c>
-      <c r="D35" s="32">
-        <f>+$E$10-($E$10-C35)/($E$13*$E$15/$E$9*LN($E$15/$E$7)+1)</f>
-        <v>21.570023593713483</v>
-      </c>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="7">
-        <v>10</v>
-      </c>
-      <c r="C36" s="22">
-        <f t="shared" ref="C36:C65" si="0">$E$10+($E$4-$E$10)/EXP(B36/($E$26*$E$21*$E$18))</f>
-        <v>89.994947375382452</v>
-      </c>
-      <c r="D36" s="32">
-        <f t="shared" ref="D36:D65" si="1">+$E$10-($E$10-C36)/($E$13*$E$15/$E$9*LN($E$15/$E$7)+1)</f>
-        <v>21.569773066087166</v>
-      </c>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="34"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="7">
-        <v>20</v>
-      </c>
-      <c r="C37" s="22">
-        <f t="shared" si="0"/>
-        <v>89.989895105334568</v>
-      </c>
-      <c r="D37" s="32">
-        <f t="shared" si="1"/>
-        <v>21.569522556041711</v>
-      </c>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="7">
-        <v>30</v>
-      </c>
-      <c r="C38" s="22">
-        <f t="shared" si="0"/>
-        <v>89.98484318983148</v>
-      </c>
-      <c r="D38" s="32">
-        <f t="shared" si="1"/>
-        <v>21.569272063575884</v>
-      </c>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="7">
-        <v>40</v>
-      </c>
-      <c r="C39" s="22">
-        <f t="shared" si="0"/>
-        <v>89.979791628848275</v>
-      </c>
-      <c r="D39" s="32">
-        <f t="shared" si="1"/>
-        <v>21.56902158868845</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="7">
-        <v>50</v>
-      </c>
-      <c r="C40" s="22">
-        <f t="shared" si="0"/>
-        <v>89.974740422360085</v>
-      </c>
-      <c r="D40" s="32">
-        <f t="shared" si="1"/>
-        <v>21.568771131378181</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="7">
-        <v>60</v>
-      </c>
-      <c r="C41" s="22">
-        <f t="shared" si="0"/>
-        <v>89.969689570342041</v>
-      </c>
-      <c r="D41" s="32">
-        <f t="shared" si="1"/>
-        <v>21.568520691643837</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="7">
-        <v>70</v>
-      </c>
-      <c r="C42" s="22">
-        <f t="shared" si="0"/>
-        <v>89.964639072769259</v>
-      </c>
-      <c r="D42" s="32">
-        <f t="shared" si="1"/>
-        <v>21.568270269484184</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="7">
-        <v>80</v>
-      </c>
-      <c r="C43" s="22">
-        <f t="shared" si="0"/>
-        <v>89.959588929616871</v>
-      </c>
-      <c r="D43" s="32">
-        <f t="shared" si="1"/>
-        <v>21.568019864897995</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="7">
-        <v>90</v>
-      </c>
-      <c r="C44" s="22">
-        <f t="shared" si="0"/>
-        <v>89.954539140860021</v>
-      </c>
-      <c r="D44" s="32">
-        <f t="shared" si="1"/>
-        <v>21.567769477884035</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="7">
-        <v>100</v>
-      </c>
-      <c r="C45" s="22">
-        <f t="shared" si="0"/>
-        <v>89.949489706473813</v>
-      </c>
-      <c r="D45" s="32">
-        <f t="shared" si="1"/>
-        <v>21.567519108441068</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="7">
-        <v>110</v>
-      </c>
-      <c r="C46" s="22">
-        <f t="shared" si="0"/>
-        <v>89.944440626433391</v>
-      </c>
-      <c r="D46" s="32">
-        <f t="shared" si="1"/>
-        <v>21.567268756567859</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="7">
-        <v>120</v>
-      </c>
-      <c r="C47" s="22">
-        <f t="shared" si="0"/>
-        <v>89.939391900713886</v>
-      </c>
-      <c r="D47" s="32">
-        <f t="shared" si="1"/>
-        <v>21.567018422263182</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="7">
-        <v>130</v>
-      </c>
-      <c r="C48" s="22">
-        <f t="shared" si="0"/>
-        <v>89.93434352929043</v>
-      </c>
-      <c r="D48" s="32">
-        <f t="shared" si="1"/>
-        <v>21.566768105525799</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="7">
-        <v>140</v>
-      </c>
-      <c r="C49" s="22">
-        <f t="shared" si="0"/>
-        <v>89.929295512138168</v>
-      </c>
-      <c r="D49" s="32">
-        <f t="shared" si="1"/>
-        <v>21.566517806354479</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="7">
-        <v>150</v>
-      </c>
-      <c r="C50" s="22">
-        <f t="shared" si="0"/>
-        <v>89.924247849232245</v>
-      </c>
-      <c r="D50" s="32">
-        <f t="shared" si="1"/>
-        <v>21.566267524747989</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="7">
-        <v>160</v>
-      </c>
-      <c r="C51" s="22">
-        <f t="shared" si="0"/>
-        <v>89.919200540547791</v>
-      </c>
-      <c r="D51" s="32">
-        <f t="shared" si="1"/>
-        <v>21.566017260705099</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="7">
-        <v>170</v>
-      </c>
-      <c r="C52" s="22">
-        <f t="shared" si="0"/>
-        <v>89.914153586059939</v>
-      </c>
-      <c r="D52" s="32">
-        <f t="shared" si="1"/>
-        <v>21.565767014224569</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="7">
-        <v>180</v>
-      </c>
-      <c r="C53" s="22">
-        <f t="shared" si="0"/>
-        <v>89.909106985743847</v>
-      </c>
-      <c r="D53" s="32">
-        <f t="shared" si="1"/>
-        <v>21.565516785305174</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="7">
-        <v>190</v>
-      </c>
-      <c r="C54" s="22">
-        <f t="shared" si="0"/>
-        <v>89.90406073957466</v>
-      </c>
-      <c r="D54" s="32">
-        <f t="shared" si="1"/>
-        <v>21.565266573945678</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="7">
-        <v>200</v>
-      </c>
-      <c r="C55" s="22">
-        <f t="shared" si="0"/>
-        <v>89.899014847527511</v>
-      </c>
-      <c r="D55" s="32">
-        <f t="shared" si="1"/>
-        <v>21.565016380144851</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="7">
-        <v>210</v>
-      </c>
-      <c r="C56" s="22">
-        <f t="shared" si="0"/>
-        <v>89.893969309577585</v>
-      </c>
-      <c r="D56" s="32">
-        <f t="shared" si="1"/>
-        <v>21.564766203901456</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="7">
-        <v>220</v>
-      </c>
-      <c r="C57" s="22">
-        <f t="shared" si="0"/>
-        <v>89.888924125700001</v>
-      </c>
-      <c r="D57" s="32">
-        <f t="shared" si="1"/>
-        <v>21.564516045214269</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="7">
-        <v>230</v>
-      </c>
-      <c r="C58" s="22">
-        <f t="shared" si="0"/>
-        <v>89.883879295869917</v>
-      </c>
-      <c r="D58" s="32">
-        <f t="shared" si="1"/>
-        <v>21.564265904082053</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="7">
-        <v>240</v>
-      </c>
-      <c r="C59" s="22">
-        <f t="shared" si="0"/>
-        <v>89.878834820062494</v>
-      </c>
-      <c r="D59" s="32">
-        <f t="shared" si="1"/>
-        <v>21.564015780503574</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="7">
-        <v>250</v>
-      </c>
-      <c r="C60" s="22">
-        <f t="shared" si="0"/>
-        <v>89.873790698252861</v>
-      </c>
-      <c r="D60" s="32">
-        <f t="shared" si="1"/>
-        <v>21.563765674477601</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="7">
-        <v>260</v>
-      </c>
-      <c r="C61" s="22">
-        <f t="shared" si="0"/>
-        <v>89.868746930416222</v>
-      </c>
-      <c r="D61" s="32">
-        <f t="shared" si="1"/>
-        <v>21.563515586002907</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="7">
-        <v>270</v>
-      </c>
-      <c r="C62" s="22">
-        <f t="shared" si="0"/>
-        <v>89.863703516527721</v>
-      </c>
-      <c r="D62" s="32">
-        <f t="shared" si="1"/>
-        <v>21.563265515078257</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="7">
-        <v>280</v>
-      </c>
-      <c r="C63" s="22">
-        <f t="shared" si="0"/>
-        <v>89.858660456562518</v>
-      </c>
-      <c r="D63" s="32">
-        <f t="shared" si="1"/>
-        <v>21.56301546170242</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="7">
-        <v>290</v>
-      </c>
-      <c r="C64" s="22">
-        <f t="shared" si="0"/>
-        <v>89.853617750495758</v>
-      </c>
-      <c r="D64" s="32">
-        <f t="shared" si="1"/>
-        <v>21.562765425874161</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="8">
-        <v>300</v>
-      </c>
-      <c r="C65" s="23">
-        <f t="shared" si="0"/>
-        <v>89.848575398302629</v>
-      </c>
-      <c r="D65" s="33">
+      <c r="D66" s="28">
         <f t="shared" si="1"/>
         <v>21.562515407592254</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="F33:H38"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F34:H38"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4249,13 +4351,13 @@
               <from>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>485775</xdr:colOff>
-                <xdr:row>12</xdr:row>
+                <xdr:row>13</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>1962150</xdr:colOff>
-                <xdr:row>13</xdr:row>
+                <xdr:row>14</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
@@ -4274,13 +4376,13 @@
               <from>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>15</xdr:row>
+                <xdr:row>16</xdr:row>
                 <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>2819400</xdr:colOff>
-                <xdr:row>15</xdr:row>
+                <xdr:row>16</xdr:row>
                 <xdr:rowOff>819150</xdr:rowOff>
               </to>
             </anchor>
@@ -4299,13 +4401,13 @@
               <from>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>18</xdr:row>
+                <xdr:row>19</xdr:row>
                 <xdr:rowOff>66675</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>2809875</xdr:colOff>
-                <xdr:row>18</xdr:row>
+                <xdr:row>19</xdr:row>
                 <xdr:rowOff>819150</xdr:rowOff>
               </to>
             </anchor>
@@ -4324,13 +4426,13 @@
               <from>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>152400</xdr:colOff>
-                <xdr:row>17</xdr:row>
+                <xdr:row>18</xdr:row>
                 <xdr:rowOff>57150</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>2695575</xdr:colOff>
-                <xdr:row>18</xdr:row>
+                <xdr:row>19</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
@@ -4349,13 +4451,13 @@
               <from>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>361950</xdr:colOff>
-                <xdr:row>21</xdr:row>
+                <xdr:row>22</xdr:row>
                 <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>2657475</xdr:colOff>
-                <xdr:row>22</xdr:row>
+                <xdr:row>23</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -4372,618 +4474,621 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92BA4D7-C808-4416-BAD2-62201144B2EE}">
-  <dimension ref="B1:M37"/>
+  <dimension ref="B1:L38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:13" s="36" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="48"/>
-      <c r="I2" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="48"/>
-    </row>
-    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:12" s="30" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="73"/>
+      <c r="D2" s="74"/>
+      <c r="H2" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="74"/>
+    </row>
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="13">
+        <v>69</v>
+      </c>
+      <c r="C4" s="12">
         <v>3000</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="I4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" s="13">
+      <c r="H4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="12">
         <v>3000</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="J4" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="14"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="14">
+        <v>4186</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="14">
+        <v>4186</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="16"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="14">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="I6" s="42">
+        <f>B27</f>
+        <v>1.9487171000000008E-2</v>
+      </c>
+      <c r="J6" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="43"/>
+      <c r="L6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="14">
+        <f>0.0054</f>
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="D7" s="94" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="31">
+        <f>C6</f>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="16"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="14">
+        <f>C6-C7</f>
+        <v>4.8599999999999997E-2</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="14">
+        <f>C8</f>
+        <v>4.8599999999999997E-2</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="16"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="15">
-        <v>4186</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="17"/>
-      <c r="I5" s="7" t="s">
+      <c r="I9" s="40">
+        <f>D27</f>
+        <v>2.022142820260342</v>
+      </c>
+      <c r="J9" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="43"/>
+      <c r="L9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="21">
+        <f>C9*PI()*C8^2*1000</f>
+        <v>5.9362529472583576</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="14">
+        <v>5</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="16"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="14">
+        <v>2</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="14">
+        <v>-30</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="16"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="14">
+        <v>5</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="14">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" s="16"/>
+    </row>
+    <row r="13" spans="2:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="14">
+        <v>-30</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="14">
+        <v>11</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="16"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="14">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="21">
+        <f>1/(2*PI()) *(1/$I$12 * LN(($I$7+I6)/$I$7)+1/($I$13*$C$6))</f>
+        <v>1.3577132446610718</v>
+      </c>
+      <c r="J14" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="K14" s="16"/>
+    </row>
+    <row r="15" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="18">
+        <v>11</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15" s="75" t="s">
+        <v>83</v>
+      </c>
+      <c r="I15" s="36">
+        <f>I4/(I5*I14)/LN((I10-I11)/(I9-I11))</f>
+        <v>5.9362529472583621</v>
+      </c>
+      <c r="J15" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="16"/>
+    </row>
+    <row r="16" spans="2:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="36">
+        <f>I15*60</f>
+        <v>356.1751768355017</v>
+      </c>
+      <c r="J16" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16" s="16"/>
+    </row>
+    <row r="17" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="18">
+        <f>I15/(2*PI()*I8^2*1000)</f>
+        <v>0.4000000000000003</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="29"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="15">
-        <v>4186</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="L5" s="17"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="15">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="17"/>
-      <c r="I6" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="52">
-        <f>B26</f>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="91" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="92" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="93" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="C20" s="21">
+        <f t="shared" ref="C20:C37" si="0">1/(2*PI()) *(1/$C$14 * LN(($C$6+B20)/$C$6)+1/($C$15*$C$6))</f>
+        <v>0.86883253757813839</v>
+      </c>
+      <c r="D20" s="17">
+        <f>$C$13+($C$12-$C$13)/EXP(($C$4/($C$10*$C$5*C20)))</f>
+        <v>0.45935770588402391</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="33">
+        <f>B20*1.1</f>
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="C21" s="21">
+        <f t="shared" si="0"/>
+        <v>0.92366738037408713</v>
+      </c>
+      <c r="D21" s="17">
+        <f t="shared" ref="D21:D37" si="1">$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C21)))</f>
+        <v>0.71166385007494881</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="33">
+        <f t="shared" ref="B22:B37" si="2">B21*1.1</f>
+        <v>1.2100000000000001E-2</v>
+      </c>
+      <c r="C22" s="21">
+        <f t="shared" si="0"/>
+        <v>0.98301971394932308</v>
+      </c>
+      <c r="D22" s="17">
+        <f t="shared" si="1"/>
+        <v>0.95498940751188144</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="33">
+        <f t="shared" si="2"/>
+        <v>1.3310000000000002E-2</v>
+      </c>
+      <c r="C23" s="21">
+        <f t="shared" si="0"/>
+        <v>1.047177077445451</v>
+      </c>
+      <c r="D23" s="17">
+        <f t="shared" si="1"/>
+        <v>1.1887866479532505</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="33">
+        <f t="shared" si="2"/>
+        <v>1.4641000000000003E-2</v>
+      </c>
+      <c r="C24" s="21">
+        <f t="shared" si="0"/>
+        <v>1.1164314404201443</v>
+      </c>
+      <c r="D24" s="17">
+        <f t="shared" si="1"/>
+        <v>1.4126365692856382</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="33">
+        <f t="shared" si="2"/>
+        <v>1.6105100000000004E-2</v>
+      </c>
+      <c r="C25" s="21">
+        <f t="shared" si="0"/>
+        <v>1.1910769505621619</v>
+      </c>
+      <c r="D25" s="17">
+        <f t="shared" si="1"/>
+        <v>1.6262449487694006</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="33">
+        <f t="shared" si="2"/>
+        <v>1.7715610000000007E-2</v>
+      </c>
+      <c r="C26" s="21">
+        <f t="shared" si="0"/>
+        <v>1.2714073735247722</v>
+      </c>
+      <c r="D26" s="17">
+        <f t="shared" si="1"/>
+        <v>1.8294358083716062</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="33">
+        <f t="shared" si="2"/>
         <v>1.9487171000000008E-2</v>
       </c>
-      <c r="K6" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="53"/>
-      <c r="M6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="15">
-        <f>0.1*C6</f>
-        <v>5.4000000000000003E-3</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="17"/>
-      <c r="I7" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="37">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="K7" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="17"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="17"/>
-      <c r="I8" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="J8" s="15">
-        <f>0.05</f>
-        <v>0.05</v>
-      </c>
-      <c r="K8" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="17"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="15">
-        <v>0.8</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="I9" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="50">
-        <f>D26</f>
-        <v>2.1797527235016574</v>
-      </c>
-      <c r="K9" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="L9" s="53"/>
-      <c r="M9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="22">
-        <f>C9*PI()*C8^2*1000</f>
-        <v>6.2831853071795871</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="17"/>
-      <c r="I10" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="J10" s="15">
-        <v>5</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="L10" s="17"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="15">
-        <v>2</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="I11" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="J11" s="15">
-        <v>-30</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="L11" s="17"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="15">
-        <v>5</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="17"/>
-      <c r="I12" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="J12" s="15">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="L12" s="17"/>
-    </row>
-    <row r="13" spans="2:13" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="15">
-        <v>-30</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="17"/>
-      <c r="I13" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="J13" s="15">
-        <v>11</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="L13" s="17"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="15">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="17"/>
-      <c r="I14" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="J14" s="22">
-        <f>1/(2*PI()) *(1/$J$12 * LN(($J$7+J6)/$J$7)+1/($J$13*$C$6))</f>
+      <c r="C27" s="21">
+        <f t="shared" si="0"/>
         <v>1.3577132446610718</v>
       </c>
-      <c r="K14" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="L14" s="17"/>
-    </row>
-    <row r="15" spans="2:13" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="19">
-        <v>11</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="35"/>
-      <c r="I15" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" s="43">
-        <f>J4/(J5*J14)/LN((J10-J11)/(J9-J11))</f>
-        <v>6.2831853071795853</v>
-      </c>
-      <c r="K15" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="L15" s="17"/>
-    </row>
-    <row r="16" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="43">
-        <f>J15*60</f>
-        <v>376.99111843077515</v>
-      </c>
-      <c r="K16" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="L16" s="17"/>
-    </row>
-    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I17" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="J17" s="19">
-        <f>J15/(2*PI()*J8^2*1000)</f>
-        <v>0.39999999999999991</v>
-      </c>
-      <c r="K17" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="L17" s="35"/>
-    </row>
-    <row r="18" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="39">
-        <v>0.01</v>
-      </c>
-      <c r="C19" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B19)/$C$6)+1/($C$15*$C$6))</f>
-        <v>0.86883253757813839</v>
-      </c>
-      <c r="D19" s="18">
-        <f>$C$13+($C$12-$C$13)/EXP(($C$4/($C$10*$C$5*C19)))</f>
-        <v>0.69395682249255231</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="39">
-        <f>B19*1.1</f>
-        <v>1.1000000000000001E-2</v>
-      </c>
-      <c r="C20" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B20)/$C$6)+1/($C$15*$C$6))</f>
-        <v>0.92366738037408713</v>
-      </c>
-      <c r="D20" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C20)))</f>
-        <v>0.93411282856927969</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="39">
-        <f t="shared" ref="B21:B36" si="0">B20*1.1</f>
-        <v>1.2100000000000001E-2</v>
-      </c>
-      <c r="C21" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B21)/$C$6)+1/($C$15*$C$6))</f>
-        <v>0.98301971394932308</v>
-      </c>
-      <c r="D21" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C21)))</f>
-        <v>1.1656175401129651</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="39">
-        <f t="shared" si="0"/>
-        <v>1.3310000000000002E-2</v>
-      </c>
-      <c r="C22" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B22)/$C$6)+1/($C$15*$C$6))</f>
-        <v>1.047177077445451</v>
-      </c>
-      <c r="D22" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C22)))</f>
-        <v>1.3879621776486921</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="39">
-        <f t="shared" si="0"/>
-        <v>1.4641000000000003E-2</v>
-      </c>
-      <c r="C23" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B23)/$C$6)+1/($C$15*$C$6))</f>
-        <v>1.1164314404201443</v>
-      </c>
-      <c r="D23" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C23)))</f>
-        <v>1.6007605342589386</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="39">
-        <f t="shared" si="0"/>
-        <v>1.6105100000000004E-2</v>
-      </c>
-      <c r="C24" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B24)/$C$6)+1/($C$15*$C$6))</f>
-        <v>1.1910769505621619</v>
-      </c>
-      <c r="D24" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C24)))</f>
-        <v>1.8037449117320712</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="39">
-        <f t="shared" si="0"/>
-        <v>1.7715610000000007E-2</v>
-      </c>
-      <c r="C25" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B25)/$C$6)+1/($C$15*$C$6))</f>
-        <v>1.2714073735247722</v>
-      </c>
-      <c r="D25" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C25)))</f>
-        <v>1.9967596456900338</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="39">
-        <f t="shared" si="0"/>
-        <v>1.9487171000000008E-2</v>
-      </c>
-      <c r="C26" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B26)/$C$6)+1/($C$15*$C$6))</f>
-        <v>1.3577132446610718</v>
-      </c>
-      <c r="D26" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C26)))</f>
-        <v>2.1797527235016574</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="39">
-        <f t="shared" si="0"/>
+      <c r="D27" s="17">
+        <f t="shared" si="1"/>
+        <v>2.022142820260342</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="33">
+        <f t="shared" si="2"/>
         <v>2.1435888100000012E-2</v>
       </c>
-      <c r="C27" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B27)/$C$6)+1/($C$15*$C$6))</f>
+      <c r="C28" s="21">
+        <f t="shared" si="0"/>
         <v>1.4502787657970759</v>
       </c>
-      <c r="D27" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C27)))</f>
-        <v>2.35276600758813</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="39">
-        <f t="shared" si="0"/>
+      <c r="D28" s="17">
+        <f t="shared" si="1"/>
+        <v>2.2043991913208529</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="33">
+        <f t="shared" si="2"/>
         <v>2.3579476910000015E-2</v>
       </c>
-      <c r="C28" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B28)/$C$6)+1/($C$15*$C$6))</f>
+      <c r="C29" s="21">
+        <f t="shared" si="0"/>
         <v>1.5493784943531745</v>
       </c>
-      <c r="D28" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C28)))</f>
-        <v>2.5159245569098445</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="39">
-        <f t="shared" si="0"/>
+      <c r="D29" s="17">
+        <f t="shared" si="1"/>
+        <v>2.3763265475735622</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="33">
+        <f t="shared" si="2"/>
         <v>2.5937424601000018E-2</v>
       </c>
-      <c r="C29" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B29)/$C$6)+1/($C$15*$C$6))</f>
+      <c r="C30" s="21">
+        <f t="shared" si="0"/>
         <v>1.655273886400461</v>
       </c>
-      <c r="D29" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C29)))</f>
-        <v>2.6694254976078895</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="39">
-        <f t="shared" si="0"/>
+      <c r="D30" s="17">
+        <f t="shared" si="1"/>
+        <v>2.5381232975113477</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="33">
+        <f t="shared" si="2"/>
         <v>2.8531167061100021E-2</v>
       </c>
-      <c r="C30" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B30)/$C$6)+1/($C$15*$C$6))</f>
+      <c r="C31" s="21">
+        <f t="shared" si="0"/>
         <v>1.7682097687319536</v>
       </c>
-      <c r="D30" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C30)))</f>
-        <v>2.8135268369001594</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="39">
-        <f t="shared" si="0"/>
+      <c r="D31" s="17">
+        <f t="shared" si="1"/>
+        <v>2.6900528949362155</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="33">
+        <f t="shared" si="2"/>
         <v>3.1384283767210024E-2</v>
       </c>
-      <c r="C31" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B31)/$C$6)+1/($C$15*$C$6))</f>
+      <c r="C32" s="21">
+        <f t="shared" si="0"/>
         <v>1.8884108267436404</v>
       </c>
-      <c r="D31" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C31)))</f>
-        <v>2.9485365489624655</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="39">
-        <f t="shared" si="0"/>
+      <c r="D32" s="17">
+        <f t="shared" si="1"/>
+        <v>2.8324323538361398</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="33">
+        <f t="shared" si="2"/>
         <v>3.4522712143931031E-2</v>
       </c>
-      <c r="C32" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B32)/$C$6)+1/($C$15*$C$6))</f>
+      <c r="C33" s="21">
+        <f t="shared" si="0"/>
         <v>2.0160782038214338</v>
       </c>
-      <c r="D32" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C32)))</f>
-        <v>3.074802193351978</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="39">
-        <f t="shared" si="0"/>
+      <c r="D33" s="17">
+        <f t="shared" si="1"/>
+        <v>2.9656212962961561</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="33">
+        <f t="shared" si="2"/>
         <v>3.7974983358324138E-2</v>
       </c>
-      <c r="C33" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B33)/$C$6)+1/($C$15*$C$6))</f>
+      <c r="C34" s="21">
+        <f t="shared" si="0"/>
         <v>2.1513863130398785</v>
       </c>
-      <c r="D33" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C33)))</f>
-        <v>3.1927012601055154</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="39">
-        <f t="shared" si="0"/>
+      <c r="D34" s="17">
+        <f t="shared" si="1"/>
+        <v>3.0900117443007176</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="33">
+        <f t="shared" si="2"/>
         <v>4.1772481694156552E-2</v>
       </c>
-      <c r="C34" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B34)/$C$6)+1/($C$15*$C$6))</f>
+      <c r="C35" s="21">
+        <f t="shared" si="0"/>
         <v>2.2944799624836016</v>
       </c>
-      <c r="D34" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C34)))</f>
-        <v>3.3026323742934807</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="39">
-        <f t="shared" si="0"/>
+      <c r="D35" s="17">
+        <f t="shared" si="1"/>
+        <v>3.2060188011793471</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="33">
+        <f t="shared" si="2"/>
         <v>4.5949729863572208E-2</v>
       </c>
-      <c r="C35" s="22">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B35)/$C$6)+1/($C$15*$C$6))</f>
+      <c r="C36" s="21">
+        <f t="shared" si="0"/>
         <v>2.4454718908623758</v>
       </c>
-      <c r="D35" s="18">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C35)))</f>
-        <v>3.4050074386848479</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="44">
-        <f t="shared" si="0"/>
+      <c r="D36" s="17">
+        <f t="shared" si="1"/>
+        <v>3.3140723107566643</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="37">
+        <f t="shared" si="2"/>
         <v>5.0544702849929436E-2</v>
       </c>
-      <c r="C36" s="23">
-        <f>1/(2*PI()) *(1/$C$14 * LN(($C$6+B36)/$C$6)+1/($C$15*$C$6))</f>
+      <c r="C37" s="22">
+        <f t="shared" si="0"/>
         <v>2.6044408001280686</v>
       </c>
-      <c r="D36" s="24">
-        <f>$C$13+($C$12-$C$13)*EXP(-($C$4/($C$10*$C$5*C36)))</f>
-        <v>3.5002447474108536</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
+      <c r="D37" s="23">
+        <f t="shared" si="1"/>
+        <v>3.4146095332783588</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="B2:D2"/>
   </mergeCells>
-  <conditionalFormatting sqref="D19:D36">
+  <conditionalFormatting sqref="D20:D37">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>$C$11</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update Coibentazione delle tubazioni.xlsx
</commit_message>
<xml_diff>
--- a/FogliCalcolo/Piping/Coibentazione delle tubazioni.xlsx
+++ b/FogliCalcolo/Piping/Coibentazione delle tubazioni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giona\Desktop\git\ImpiantiMeccanici\FogliCalcolo\Piping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A1BFDC-6AD5-41D2-A65D-695D6CBDAD64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6A81B9-5A8F-47AE-89DD-55347F34E6C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -771,75 +771,6 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -859,6 +790,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
@@ -2999,7 +2999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B19" sqref="B19:B44"/>
     </sheetView>
   </sheetViews>
@@ -3018,10 +3018,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="70"/>
+      <c r="E2" s="87"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
@@ -3031,7 +3031,7 @@
       <c r="D3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="92">
+      <c r="E3" s="69">
         <v>5</v>
       </c>
     </row>
@@ -3043,7 +3043,7 @@
       <c r="D4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="93">
+      <c r="E4" s="70">
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
@@ -3055,7 +3055,7 @@
       <c r="D5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="92">
+      <c r="E5" s="69">
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
@@ -3090,7 +3090,7 @@
       <c r="D8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="92">
+      <c r="E8" s="69">
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
@@ -3102,7 +3102,7 @@
       <c r="D9" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="92">
+      <c r="E9" s="69">
         <v>35</v>
       </c>
     </row>
@@ -3112,7 +3112,7 @@
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="15"/>
-      <c r="E10" s="94">
+      <c r="E10" s="71">
         <v>0.8</v>
       </c>
     </row>
@@ -3122,7 +3122,7 @@
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="15"/>
-      <c r="E11" s="92">
+      <c r="E11" s="69">
         <v>31</v>
       </c>
     </row>
@@ -3147,7 +3147,7 @@
       <c r="D13" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="95">
+      <c r="E13" s="72">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="F13" s="63" t="s">
@@ -3198,7 +3198,7 @@
       <c r="E18" s="13"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="96">
+      <c r="B19" s="73">
         <v>0.01</v>
       </c>
       <c r="C19" s="50">
@@ -3215,7 +3215,7 @@
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="96">
+      <c r="B20" s="73">
         <v>1.2E-2</v>
       </c>
       <c r="C20" s="50">
@@ -3232,7 +3232,7 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="96">
+      <c r="B21" s="73">
         <v>1.4E-2</v>
       </c>
       <c r="C21" s="50">
@@ -3249,7 +3249,7 @@
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="96">
+      <c r="B22" s="73">
         <v>1.6E-2</v>
       </c>
       <c r="C22" s="50">
@@ -3266,7 +3266,7 @@
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="96">
+      <c r="B23" s="73">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="C23" s="50">
@@ -3283,7 +3283,7 @@
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="96">
+      <c r="B24" s="73">
         <v>0.02</v>
       </c>
       <c r="C24" s="50">
@@ -3300,7 +3300,7 @@
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="96">
+      <c r="B25" s="73">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="C25" s="50">
@@ -3317,7 +3317,7 @@
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="96">
+      <c r="B26" s="73">
         <v>2.4E-2</v>
       </c>
       <c r="C26" s="50">
@@ -3334,7 +3334,7 @@
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="96">
+      <c r="B27" s="73">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="C27" s="50">
@@ -3351,7 +3351,7 @@
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="96">
+      <c r="B28" s="73">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="C28" s="50">
@@ -3369,7 +3369,7 @@
       <c r="F28" s="54"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="96">
+      <c r="B29" s="73">
         <v>0.03</v>
       </c>
       <c r="C29" s="50">
@@ -3386,7 +3386,7 @@
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="96">
+      <c r="B30" s="73">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="C30" s="50">
@@ -3403,7 +3403,7 @@
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="96">
+      <c r="B31" s="73">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="C31" s="50">
@@ -3420,7 +3420,7 @@
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="96">
+      <c r="B32" s="73">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="C32" s="50">
@@ -3437,7 +3437,7 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="96">
+      <c r="B33" s="73">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="C33" s="50">
@@ -3454,7 +3454,7 @@
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="96">
+      <c r="B34" s="73">
         <v>0.04</v>
       </c>
       <c r="C34" s="50">
@@ -3471,7 +3471,7 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="96">
+      <c r="B35" s="73">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="C35" s="50">
@@ -3488,7 +3488,7 @@
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="96">
+      <c r="B36" s="73">
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="C36" s="50">
@@ -3505,7 +3505,7 @@
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="96">
+      <c r="B37" s="73">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="C37" s="50">
@@ -3522,7 +3522,7 @@
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="96">
+      <c r="B38" s="73">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="C38" s="50">
@@ -3539,7 +3539,7 @@
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="96">
+      <c r="B39" s="73">
         <v>0.05</v>
       </c>
       <c r="C39" s="50">
@@ -3556,7 +3556,7 @@
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="96">
+      <c r="B40" s="73">
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="C40" s="50">
@@ -3574,7 +3574,7 @@
       <c r="F40" s="14"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="96">
+      <c r="B41" s="73">
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="C41" s="50">
@@ -3591,7 +3591,7 @@
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="96">
+      <c r="B42" s="73">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="C42" s="50">
@@ -3608,7 +3608,7 @@
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="96">
+      <c r="B43" s="73">
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="C43" s="50">
@@ -3625,7 +3625,7 @@
       </c>
     </row>
     <row r="44" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="97">
+      <c r="B44" s="74">
         <v>0.06</v>
       </c>
       <c r="C44" s="51">
@@ -3720,7 +3720,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
@@ -3728,22 +3728,22 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="73"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="90"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="14"/>
-      <c r="D3" s="86" t="s">
+      <c r="D3" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="87"/>
+      <c r="E3" s="104"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -3753,7 +3753,7 @@
       <c r="D4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="98">
+      <c r="E4" s="75">
         <v>90</v>
       </c>
     </row>
@@ -3765,7 +3765,7 @@
       <c r="D5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="98">
+      <c r="E5" s="75">
         <v>80</v>
       </c>
     </row>
@@ -3777,7 +3777,7 @@
       <c r="D6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="93">
+      <c r="E6" s="70">
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
@@ -3789,7 +3789,7 @@
       <c r="D7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="93">
+      <c r="E7" s="70">
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
@@ -3811,10 +3811,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="14"/>
-      <c r="D9" s="86" t="s">
+      <c r="D9" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="87"/>
+      <c r="E9" s="104"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
@@ -3824,7 +3824,7 @@
       <c r="D10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="92">
+      <c r="E10" s="69">
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
@@ -3836,7 +3836,7 @@
       <c r="D11" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="98">
+      <c r="E11" s="75">
         <v>18</v>
       </c>
     </row>
@@ -3846,7 +3846,7 @@
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="15"/>
-      <c r="E12" s="94">
+      <c r="E12" s="71">
         <v>0.5</v>
       </c>
     </row>
@@ -3856,7 +3856,7 @@
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="15"/>
-      <c r="E13" s="92">
+      <c r="E13" s="69">
         <v>13</v>
       </c>
     </row>
@@ -3881,7 +3881,7 @@
       <c r="D15" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="99">
+      <c r="E15" s="76">
         <v>0.06</v>
       </c>
     </row>
@@ -3919,7 +3919,7 @@
       <c r="D18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="92">
+      <c r="E18" s="69">
         <v>300</v>
       </c>
     </row>
@@ -3957,7 +3957,7 @@
       <c r="D21" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="100">
+      <c r="E21" s="77">
         <v>1.5</v>
       </c>
     </row>
@@ -4071,16 +4071,16 @@
     </row>
     <row r="33" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="74" t="s">
+      <c r="B34" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="75"/>
-      <c r="D34" s="76"/>
-      <c r="F34" s="77" t="s">
+      <c r="C34" s="92"/>
+      <c r="D34" s="93"/>
+      <c r="F34" s="94" t="s">
         <v>51</v>
       </c>
-      <c r="G34" s="78"/>
-      <c r="H34" s="79"/>
+      <c r="G34" s="95"/>
+      <c r="H34" s="96"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="27" t="s">
@@ -4092,12 +4092,12 @@
       <c r="D35" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F35" s="80"/>
-      <c r="G35" s="81"/>
-      <c r="H35" s="82"/>
+      <c r="F35" s="97"/>
+      <c r="G35" s="98"/>
+      <c r="H35" s="99"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="101">
+      <c r="B36" s="78">
         <v>0</v>
       </c>
       <c r="C36" s="21">
@@ -4108,12 +4108,12 @@
         <f>+$E$11-($E$11-C36)/($E$14*$E$16/$E$10*LN($E$16/$E$6)+1)</f>
         <v>21.570023593713483</v>
       </c>
-      <c r="F36" s="80"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="82"/>
+      <c r="F36" s="97"/>
+      <c r="G36" s="98"/>
+      <c r="H36" s="99"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="101">
+      <c r="B37" s="78">
         <v>10</v>
       </c>
       <c r="C37" s="21">
@@ -4124,12 +4124,12 @@
         <f t="shared" ref="D37:D66" si="1">+$E$11-($E$11-C37)/($E$14*$E$16/$E$10*LN($E$16/$E$6)+1)</f>
         <v>21.569773066087166</v>
       </c>
-      <c r="F37" s="80"/>
-      <c r="G37" s="81"/>
-      <c r="H37" s="82"/>
+      <c r="F37" s="97"/>
+      <c r="G37" s="98"/>
+      <c r="H37" s="99"/>
     </row>
     <row r="38" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="101">
+      <c r="B38" s="78">
         <v>20</v>
       </c>
       <c r="C38" s="21">
@@ -4140,12 +4140,12 @@
         <f t="shared" si="1"/>
         <v>21.569522556041711</v>
       </c>
-      <c r="F38" s="83"/>
-      <c r="G38" s="84"/>
-      <c r="H38" s="85"/>
+      <c r="F38" s="100"/>
+      <c r="G38" s="101"/>
+      <c r="H38" s="102"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="101">
+      <c r="B39" s="78">
         <v>30</v>
       </c>
       <c r="C39" s="21">
@@ -4161,7 +4161,7 @@
       <c r="H39" s="55"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="101">
+      <c r="B40" s="78">
         <v>40</v>
       </c>
       <c r="C40" s="21">
@@ -4174,7 +4174,7 @@
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="101">
+      <c r="B41" s="78">
         <v>50</v>
       </c>
       <c r="C41" s="21">
@@ -4187,7 +4187,7 @@
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="101">
+      <c r="B42" s="78">
         <v>60</v>
       </c>
       <c r="C42" s="21">
@@ -4200,7 +4200,7 @@
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="101">
+      <c r="B43" s="78">
         <v>70</v>
       </c>
       <c r="C43" s="21">
@@ -4213,7 +4213,7 @@
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="101">
+      <c r="B44" s="78">
         <v>80</v>
       </c>
       <c r="C44" s="21">
@@ -4226,7 +4226,7 @@
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="101">
+      <c r="B45" s="78">
         <v>90</v>
       </c>
       <c r="C45" s="21">
@@ -4239,7 +4239,7 @@
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="101">
+      <c r="B46" s="78">
         <v>100</v>
       </c>
       <c r="C46" s="21">
@@ -4252,7 +4252,7 @@
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="101">
+      <c r="B47" s="78">
         <v>110</v>
       </c>
       <c r="C47" s="21">
@@ -4265,7 +4265,7 @@
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="101">
+      <c r="B48" s="78">
         <v>120</v>
       </c>
       <c r="C48" s="21">
@@ -4278,7 +4278,7 @@
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="101">
+      <c r="B49" s="78">
         <v>130</v>
       </c>
       <c r="C49" s="21">
@@ -4291,7 +4291,7 @@
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="101">
+      <c r="B50" s="78">
         <v>140</v>
       </c>
       <c r="C50" s="21">
@@ -4304,7 +4304,7 @@
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="101">
+      <c r="B51" s="78">
         <v>150</v>
       </c>
       <c r="C51" s="21">
@@ -4317,7 +4317,7 @@
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="101">
+      <c r="B52" s="78">
         <v>160</v>
       </c>
       <c r="C52" s="21">
@@ -4330,7 +4330,7 @@
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="101">
+      <c r="B53" s="78">
         <v>170</v>
       </c>
       <c r="C53" s="21">
@@ -4343,7 +4343,7 @@
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="101">
+      <c r="B54" s="78">
         <v>180</v>
       </c>
       <c r="C54" s="21">
@@ -4356,7 +4356,7 @@
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="101">
+      <c r="B55" s="78">
         <v>190</v>
       </c>
       <c r="C55" s="21">
@@ -4369,7 +4369,7 @@
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="101">
+      <c r="B56" s="78">
         <v>200</v>
       </c>
       <c r="C56" s="21">
@@ -4382,7 +4382,7 @@
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="101">
+      <c r="B57" s="78">
         <v>210</v>
       </c>
       <c r="C57" s="21">
@@ -4395,7 +4395,7 @@
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="101">
+      <c r="B58" s="78">
         <v>220</v>
       </c>
       <c r="C58" s="21">
@@ -4408,7 +4408,7 @@
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="101">
+      <c r="B59" s="78">
         <v>230</v>
       </c>
       <c r="C59" s="21">
@@ -4421,7 +4421,7 @@
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="101">
+      <c r="B60" s="78">
         <v>240</v>
       </c>
       <c r="C60" s="21">
@@ -4434,7 +4434,7 @@
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="101">
+      <c r="B61" s="78">
         <v>250</v>
       </c>
       <c r="C61" s="21">
@@ -4447,7 +4447,7 @@
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="101">
+      <c r="B62" s="78">
         <v>260</v>
       </c>
       <c r="C62" s="21">
@@ -4460,7 +4460,7 @@
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="101">
+      <c r="B63" s="78">
         <v>270</v>
       </c>
       <c r="C63" s="21">
@@ -4473,7 +4473,7 @@
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="101">
+      <c r="B64" s="78">
         <v>280</v>
       </c>
       <c r="C64" s="21">
@@ -4486,7 +4486,7 @@
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="101">
+      <c r="B65" s="78">
         <v>290</v>
       </c>
       <c r="C65" s="21">
@@ -4499,7 +4499,7 @@
       </c>
     </row>
     <row r="66" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="102">
+      <c r="B66" s="79">
         <v>300</v>
       </c>
       <c r="C66" s="22">
@@ -4658,7 +4658,7 @@
   <dimension ref="B1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4671,24 +4671,24 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="30" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="90"/>
-      <c r="H2" s="88" t="s">
+      <c r="C2" s="106"/>
+      <c r="D2" s="107"/>
+      <c r="H2" s="105" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="90"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="107"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="103">
+      <c r="C4" s="80">
         <v>3000</v>
       </c>
       <c r="D4" s="13" t="s">
@@ -4697,7 +4697,7 @@
       <c r="H4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="106">
+      <c r="I4" s="83">
         <f>C4</f>
         <v>3000</v>
       </c>
@@ -4732,7 +4732,7 @@
       <c r="B6" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="104">
+      <c r="C6" s="81">
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="D6" s="16" t="s">
@@ -4741,7 +4741,7 @@
       <c r="H6" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="107">
+      <c r="I6" s="84">
         <v>1.9E-2</v>
       </c>
       <c r="J6" s="38" t="s">
@@ -4753,7 +4753,7 @@
       <c r="B7" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="104">
+      <c r="C7" s="81">
         <f>0.0054</f>
         <v>5.4000000000000003E-3</v>
       </c>
@@ -4799,7 +4799,7 @@
       <c r="B9" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="104">
+      <c r="C9" s="81">
         <v>0.8</v>
       </c>
       <c r="D9" s="16" t="s">
@@ -4808,7 +4808,7 @@
       <c r="H9" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="108">
+      <c r="I9" s="85">
         <v>2.02</v>
       </c>
       <c r="J9" s="38" t="s">
@@ -4843,7 +4843,7 @@
       <c r="B11" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="104">
+      <c r="C11" s="81">
         <v>2</v>
       </c>
       <c r="D11" s="16" t="s">
@@ -4865,7 +4865,7 @@
       <c r="B12" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="104">
+      <c r="C12" s="81">
         <v>5</v>
       </c>
       <c r="D12" s="16" t="s">
@@ -4887,7 +4887,7 @@
       <c r="B13" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="104">
+      <c r="C13" s="81">
         <v>-30</v>
       </c>
       <c r="D13" s="16" t="s">
@@ -4909,7 +4909,7 @@
       <c r="B14" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="104">
+      <c r="C14" s="81">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="D14" s="16" t="s">
@@ -4931,13 +4931,13 @@
       <c r="B15" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="105">
+      <c r="C15" s="82">
         <v>11</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="H15" s="91" t="s">
+      <c r="H15" s="108" t="s">
         <v>80</v>
       </c>
       <c r="I15" s="35">
@@ -4953,7 +4953,7 @@
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
-      <c r="H16" s="91"/>
+      <c r="H16" s="108"/>
       <c r="I16" s="35">
         <f>I15*60</f>
         <v>362.1827208148207</v>
@@ -5007,7 +5007,7 @@
       <c r="K19" s="14"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="96">
+      <c r="B20" s="73">
         <v>0.01</v>
       </c>
       <c r="C20" s="21">
@@ -5020,7 +5020,7 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="96">
+      <c r="B21" s="73">
         <f>B20*1.1</f>
         <v>1.1000000000000001E-2</v>
       </c>
@@ -5034,7 +5034,7 @@
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="96">
+      <c r="B22" s="73">
         <f t="shared" ref="B22:B37" si="2">B21*1.1</f>
         <v>1.2100000000000001E-2</v>
       </c>
@@ -5048,7 +5048,7 @@
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="96">
+      <c r="B23" s="73">
         <f t="shared" si="2"/>
         <v>1.3310000000000002E-2</v>
       </c>
@@ -5062,7 +5062,7 @@
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="96">
+      <c r="B24" s="73">
         <f t="shared" si="2"/>
         <v>1.4641000000000003E-2</v>
       </c>
@@ -5076,7 +5076,7 @@
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="96">
+      <c r="B25" s="73">
         <f t="shared" si="2"/>
         <v>1.6105100000000004E-2</v>
       </c>
@@ -5090,7 +5090,7 @@
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="96">
+      <c r="B26" s="73">
         <f t="shared" si="2"/>
         <v>1.7715610000000007E-2</v>
       </c>
@@ -5104,7 +5104,7 @@
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="96">
+      <c r="B27" s="73">
         <f t="shared" si="2"/>
         <v>1.9487171000000008E-2</v>
       </c>
@@ -5118,7 +5118,7 @@
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="96">
+      <c r="B28" s="73">
         <f t="shared" si="2"/>
         <v>2.1435888100000012E-2</v>
       </c>
@@ -5132,7 +5132,7 @@
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="96">
+      <c r="B29" s="73">
         <f t="shared" si="2"/>
         <v>2.3579476910000015E-2</v>
       </c>
@@ -5146,7 +5146,7 @@
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="96">
+      <c r="B30" s="73">
         <f t="shared" si="2"/>
         <v>2.5937424601000018E-2</v>
       </c>
@@ -5160,7 +5160,7 @@
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="96">
+      <c r="B31" s="73">
         <f t="shared" si="2"/>
         <v>2.8531167061100021E-2</v>
       </c>
@@ -5174,7 +5174,7 @@
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="96">
+      <c r="B32" s="73">
         <f t="shared" si="2"/>
         <v>3.1384283767210024E-2</v>
       </c>
@@ -5188,7 +5188,7 @@
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="96">
+      <c r="B33" s="73">
         <f t="shared" si="2"/>
         <v>3.4522712143931031E-2</v>
       </c>
@@ -5202,7 +5202,7 @@
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="96">
+      <c r="B34" s="73">
         <f t="shared" si="2"/>
         <v>3.7974983358324138E-2</v>
       </c>
@@ -5216,7 +5216,7 @@
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="96">
+      <c r="B35" s="73">
         <f t="shared" si="2"/>
         <v>4.1772481694156552E-2</v>
       </c>
@@ -5230,7 +5230,7 @@
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="96">
+      <c r="B36" s="73">
         <f t="shared" si="2"/>
         <v>4.5949729863572208E-2</v>
       </c>
@@ -5244,7 +5244,7 @@
       </c>
     </row>
     <row r="37" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="97">
+      <c r="B37" s="74">
         <f t="shared" si="2"/>
         <v>5.0544702849929436E-2</v>
       </c>

</xml_diff>